<commit_message>
Adding initial conditions file to appendices subdir
</commit_message>
<xml_diff>
--- a/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
+++ b/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
   <si>
     <r>
       <t>__</t>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>4.5/4.5/4.8</t>
+  </si>
+  <si>
+    <t>After severe protein permeability and 1 week</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>After GFR lowered and 1 week</t>
   </si>
 </sst>
 </file>
@@ -545,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,7 +569,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:18" ht="30.75" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -571,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30.75" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -581,19 +590,22 @@
       <c r="C4" s="5">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="45.75" thickBot="1">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="75.75" thickBot="1">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -605,7 +617,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:18" ht="45.75" thickBot="1">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -616,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30.75" thickBot="1">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -626,8 +638,11 @@
       <c r="C9" s="5">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="45.75" thickBot="1">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="30.75" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -691,6 +706,9 @@
       <c r="C15" s="5">
         <v>2.2690000000000001</v>
       </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:18" ht="30.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -703,7 +721,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30.75" thickBot="1">
+    <row r="17" spans="1:4" ht="30.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -714,7 +732,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30.75" thickBot="1">
+    <row r="18" spans="1:4" ht="30.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -725,8 +743,8 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
         <v>2</v>
@@ -735,7 +753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30.75" thickBot="1">
+    <row r="21" spans="1:4" ht="30.75" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
@@ -745,8 +763,11 @@
       <c r="C21" s="5">
         <v>3.3580000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30.75" thickBot="1">
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30.75" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
@@ -757,7 +778,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30.75" thickBot="1">
+    <row r="23" spans="1:4" ht="30.75" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
@@ -768,7 +789,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30.75" thickBot="1">
+    <row r="24" spans="1:4" ht="30.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -779,8 +800,8 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:3" ht="30.75" thickBot="1">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="26" spans="1:4" ht="30.75" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -791,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+    <row r="27" spans="1:4" ht="15.75" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -802,8 +823,8 @@
         <v>2754</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
         <v>2</v>
@@ -812,7 +833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30.75" thickBot="1">
+    <row r="30" spans="1:4" ht="30.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
@@ -823,7 +844,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30.75" thickBot="1">
+    <row r="31" spans="1:4" ht="30.75" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -834,7 +855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30.75" thickBot="1">
+    <row r="32" spans="1:4" ht="30.75" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Adding HumMod Data to Lab 31
</commit_message>
<xml_diff>
--- a/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
+++ b/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
   <si>
     <t>Plasma Protein</t>
   </si>
@@ -112,6 +112,79 @@
   </si>
   <si>
     <t>4.4/4.4/5.3</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>After 1 week of nephrotic syndrome</t>
+  </si>
+  <si>
+    <t>2.4/2.6/ 2.8</t>
+  </si>
+  <si>
+    <t>8.5/8.9/ 9.7</t>
+  </si>
+  <si>
+    <t>HumMod also does not give protein colloid pressure or concentration for the interstitial as a whole. So insteal, Upper, Middle, and Lower Torso values have been given in that order.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.0349</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> G/Min x 1440 = </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>50.256</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> G/Day</t>
+    </r>
+  </si>
+  <si>
+    <t>1.5/1.7/ 1.8</t>
+  </si>
+  <si>
+    <t>5.0/5.8/ 6.3</t>
+  </si>
+  <si>
+    <t>These two values are very, very difficult to find in HumMod</t>
+  </si>
+  <si>
+    <t>Why is this happening?</t>
+  </si>
+  <si>
+    <t>Significant differences in multiple categories exist in this lab.</t>
   </si>
 </sst>
 </file>
@@ -154,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -214,11 +287,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -235,10 +335,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R63"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,9 +667,19 @@
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="30.75" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,8 +689,17 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -574,8 +712,17 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
+        <v>215</v>
+      </c>
+      <c r="K4" s="5">
+        <v>124.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="45.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -585,8 +732,17 @@
       <c r="C5" s="5">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="5">
+        <v>7</v>
+      </c>
+      <c r="K5" s="5">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="75.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -596,9 +752,18 @@
       <c r="C6" s="5">
         <v>19</v>
       </c>
+      <c r="I6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5">
+        <v>28</v>
+      </c>
+      <c r="K6" s="5">
+        <v>19.7</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1">
+    <row r="8" spans="1:18" ht="45.75" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -608,8 +773,17 @@
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="30.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -622,8 +796,17 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>294.8</v>
+      </c>
+      <c r="K9" s="5">
+        <v>273.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="45.75" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -633,8 +816,17 @@
       <c r="C10" s="5">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="75.75" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -644,28 +836,39 @@
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75">
-      <c r="A12" s="6" t="s">
+      <c r="I11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="109.5" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:18" ht="15.75" thickBot="1">
@@ -676,8 +879,15 @@
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I14" s="2"/>
+      <c r="J14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="45.75" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -690,8 +900,17 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="K15" s="5">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="60.75" thickBot="1">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -701,8 +920,17 @@
       <c r="C16" s="5">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="K16" s="5">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="75.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -712,8 +940,21 @@
       <c r="C17" s="5">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="30.75" thickBot="1">
+      <c r="G17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="5">
+        <v>2.72</v>
+      </c>
+      <c r="K17" s="5">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="60.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -723,9 +964,20 @@
       <c r="C18" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="5">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K18" s="5">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
         <v>1</v>
@@ -733,8 +985,15 @@
       <c r="C20" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I20" s="2"/>
+      <c r="J20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45.75" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -747,8 +1006,17 @@
       <c r="D21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="K21" s="5">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60.75" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -758,8 +1026,17 @@
       <c r="C22" s="5">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="K22" s="5">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="75.75" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
@@ -769,8 +1046,17 @@
       <c r="C23" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="5">
+        <v>2.72</v>
+      </c>
+      <c r="K23" s="5">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -780,9 +1066,18 @@
       <c r="C24" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K24" s="5">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="26" spans="1:11" ht="45.75" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -792,8 +1087,17 @@
       <c r="C26" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1">
+      <c r="I26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30.75" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -803,9 +1107,21 @@
       <c r="C27" s="5">
         <v>2611</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="5">
+        <v>2014.5</v>
+      </c>
+      <c r="K27" s="5">
+        <v>3334.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
         <v>1</v>
@@ -813,8 +1129,15 @@
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I29" s="2"/>
+      <c r="J29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="75.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -824,8 +1147,20 @@
       <c r="C30" s="5">
         <v>103</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="30.75" thickBot="1">
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="5">
+        <v>97</v>
+      </c>
+      <c r="K30" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="90.75" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -835,8 +1170,17 @@
       <c r="C31" s="5">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="30.75" thickBot="1">
+      <c r="I31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="5">
+        <v>62</v>
+      </c>
+      <c r="K31" s="5">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45.75" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -846,8 +1190,17 @@
       <c r="C32" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K32" s="5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="75.75" thickBot="1">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -857,8 +1210,17 @@
       <c r="C33" s="5">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="K33" s="5">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="30.75" thickBot="1">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
@@ -868,8 +1230,22 @@
       <c r="C34" s="5">
         <v>220</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="30.75" thickBot="1">
+      <c r="D34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="I34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="5">
+        <v>306.89999999999998</v>
+      </c>
+      <c r="K34" s="5">
+        <v>431.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="45.75" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>18</v>
       </c>
@@ -879,9 +1255,18 @@
       <c r="C35" s="5">
         <v>1.3</v>
       </c>
+      <c r="I35" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K35" s="5">
+        <v>1.29</v>
+      </c>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1">
+    <row r="37" spans="1:18" ht="30.75" thickBot="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -891,8 +1276,17 @@
       <c r="C37" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="30.75" thickBot="1">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -902,8 +1296,18 @@
       <c r="C38" s="5">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" ht="30.75" thickBot="1">
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="5">
+        <v>215</v>
+      </c>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:18" ht="45.75" thickBot="1">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -913,8 +1317,15 @@
       <c r="C39" s="5">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="5">
+        <v>7</v>
+      </c>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:18" ht="75.75" thickBot="1">
       <c r="A40" s="4" t="s">
         <v>5</v>
       </c>
@@ -924,9 +1335,16 @@
       <c r="C40" s="5">
         <v>18</v>
       </c>
+      <c r="I40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="5">
+        <v>28</v>
+      </c>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="42" spans="1:18" ht="15.75" thickBot="1">
+    <row r="42" spans="1:18" ht="45.75" thickBot="1">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
@@ -936,8 +1354,17 @@
       <c r="C42" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" ht="15.75" thickBot="1">
+      <c r="I42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="30.75" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -947,8 +1374,18 @@
       <c r="C43" s="5">
         <v>253</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="30.75" thickBot="1">
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J43" s="5">
+        <v>294.8</v>
+      </c>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:18" ht="45.75" thickBot="1">
       <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
@@ -958,8 +1395,15 @@
       <c r="C44" s="5">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" ht="30.75" thickBot="1">
+      <c r="I44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:18" ht="75.75" thickBot="1">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -969,28 +1413,37 @@
       <c r="C45" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" ht="15.75">
-      <c r="A46" s="6" t="s">
+      <c r="I45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:18" ht="109.5" customHeight="1">
+      <c r="A46" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
     </row>
     <row r="47" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="48" spans="1:18" ht="15.75" thickBot="1">
@@ -1001,8 +1454,15 @@
       <c r="C48" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I48" s="2"/>
+      <c r="J48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="45.75" thickBot="1">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
@@ -1012,8 +1472,20 @@
       <c r="C49" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="30.75" thickBot="1">
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="K49" s="5">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="60.75" thickBot="1">
       <c r="A50" s="4" t="s">
         <v>9</v>
       </c>
@@ -1023,8 +1495,17 @@
       <c r="C50" s="5">
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J50" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="K50" s="5">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="75.75" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>10</v>
       </c>
@@ -1034,8 +1515,17 @@
       <c r="C51" s="5">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="5">
+        <v>2.72</v>
+      </c>
+      <c r="K51" s="5">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="60.75" thickBot="1">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -1045,9 +1535,18 @@
       <c r="C52" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="54" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="5">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K52" s="5">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="54" spans="1:11" ht="45.75" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
@@ -1057,8 +1556,17 @@
       <c r="C54" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1">
+      <c r="I54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30.75" thickBot="1">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
@@ -1068,9 +1576,19 @@
       <c r="C55" s="5">
         <v>3061</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1">
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="5">
+        <v>2014.5</v>
+      </c>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="s">
         <v>1</v>
@@ -1078,8 +1596,15 @@
       <c r="C57" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I57" s="2"/>
+      <c r="J57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="75.75" thickBot="1">
       <c r="A58" s="4" t="s">
         <v>13</v>
       </c>
@@ -1089,8 +1614,20 @@
       <c r="C58" s="5">
         <v>99</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="30.75" thickBot="1">
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J58" s="5">
+        <v>97</v>
+      </c>
+      <c r="K58" s="5">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="90.75" thickBot="1">
       <c r="A59" s="4" t="s">
         <v>14</v>
       </c>
@@ -1100,8 +1637,17 @@
       <c r="C59" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I59" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="5">
+        <v>62</v>
+      </c>
+      <c r="K59" s="5">
+        <v>60.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="45.75" thickBot="1">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
@@ -1111,8 +1657,17 @@
       <c r="C60" s="5">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K60" s="5">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="75.75" thickBot="1">
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
@@ -1122,8 +1677,17 @@
       <c r="C61" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1">
+      <c r="I61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="K61" s="5">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30.75" thickBot="1">
       <c r="A62" s="4" t="s">
         <v>17</v>
       </c>
@@ -1133,8 +1697,17 @@
       <c r="C62" s="5">
         <v>708</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="30.75" thickBot="1">
+      <c r="I62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="5">
+        <v>306.89999999999998</v>
+      </c>
+      <c r="K62" s="5">
+        <v>499.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="45.75" thickBot="1">
       <c r="A63" s="4" t="s">
         <v>18</v>
       </c>
@@ -1144,10 +1717,43 @@
       <c r="C63" s="5">
         <v>3.3</v>
       </c>
+      <c r="I63" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K63" s="5">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="D34:F34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding Changes to Lab 31, correcting some of the HumMod data
</commit_message>
<xml_diff>
--- a/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
+++ b/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="39">
   <si>
     <t>Plasma Protein</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Significant differences in multiple categories exist in this lab.</t>
+  </si>
+  <si>
+    <t>0.9/1.4/ 1.6</t>
+  </si>
+  <si>
+    <t>3.1/4.7/ 5.5</t>
   </si>
 </sst>
 </file>
@@ -336,6 +342,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -354,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,21 +853,21 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="109.5" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -940,10 +946,10 @@
       <c r="C17" s="5">
         <v>4.7</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="4" t="s">
         <v>10</v>
       </c>
@@ -964,8 +970,8 @@
       <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1230,11 +1236,11 @@
       <c r="C34" s="5">
         <v>220</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
       <c r="I34" s="4" t="s">
         <v>17</v>
       </c>
@@ -1305,7 +1311,9 @@
       <c r="J38" s="5">
         <v>215</v>
       </c>
-      <c r="K38" s="5"/>
+      <c r="K38" s="5">
+        <v>160.1</v>
+      </c>
     </row>
     <row r="39" spans="1:18" ht="45.75" thickBot="1">
       <c r="A39" s="4" t="s">
@@ -1323,7 +1331,9 @@
       <c r="J39" s="5">
         <v>7</v>
       </c>
-      <c r="K39" s="5"/>
+      <c r="K39" s="5">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
     <row r="40" spans="1:18" ht="75.75" thickBot="1">
       <c r="A40" s="4" t="s">
@@ -1341,7 +1351,9 @@
       <c r="J40" s="5">
         <v>28</v>
       </c>
-      <c r="K40" s="5"/>
+      <c r="K40" s="5">
+        <v>18.3</v>
+      </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="42" spans="1:18" ht="45.75" thickBot="1">
@@ -1383,7 +1395,9 @@
       <c r="J43" s="5">
         <v>294.8</v>
       </c>
-      <c r="K43" s="5"/>
+      <c r="K43" s="5">
+        <v>265</v>
+      </c>
     </row>
     <row r="44" spans="1:18" ht="45.75" thickBot="1">
       <c r="A44" s="4" t="s">
@@ -1401,7 +1415,9 @@
       <c r="J44" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K44" s="5"/>
+      <c r="K44" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="45" spans="1:18" ht="75.75" thickBot="1">
       <c r="A45" s="4" t="s">
@@ -1419,24 +1435,26 @@
       <c r="J45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K45" s="5"/>
+      <c r="K45" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="46" spans="1:18" ht="109.5" customHeight="1">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
@@ -1585,7 +1603,9 @@
       <c r="J55" s="5">
         <v>2014.5</v>
       </c>
-      <c r="K55" s="5"/>
+      <c r="K55" s="5">
+        <v>3395.2</v>
+      </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="57" spans="1:11" ht="15.75" thickBot="1">
@@ -1728,19 +1748,19 @@
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Reformatting Lab 31 data to include percentage differences
</commit_message>
<xml_diff>
--- a/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
+++ b/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="41">
   <si>
     <t>Plasma Protein</t>
   </si>
@@ -192,12 +192,18 @@
   <si>
     <t>3.1/4.7/ 5.5</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Percent Changes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +224,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -233,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -320,11 +333,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -364,9 +387,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -660,13 +690,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75">
@@ -684,6 +715,10 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
+      <c r="O2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="16"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -704,6 +739,15 @@
       <c r="K3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="O3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="30.75" thickBot="1">
       <c r="A4" s="4" t="s">
@@ -727,6 +771,17 @@
       <c r="K4" s="5">
         <v>124.2</v>
       </c>
+      <c r="O4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="15">
+        <f>ABS((B4-J4)/B4)</f>
+        <v>3.3653846153846152E-2</v>
+      </c>
+      <c r="Q4" s="15">
+        <f t="shared" ref="Q4:Q6" si="0">ABS((C4-K4)/C4)</f>
+        <v>0.65600000000000003</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="45.75" thickBot="1">
       <c r="A5" s="4" t="s">
@@ -747,6 +802,17 @@
       <c r="K5" s="5">
         <v>5.2</v>
       </c>
+      <c r="O5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="15">
+        <f t="shared" ref="P5:P6" si="1">ABS((B5-J5)/B5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <f t="shared" si="0"/>
+        <v>6.1224489795918324E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="75.75" thickBot="1">
       <c r="A6" s="4" t="s">
@@ -766,6 +832,17 @@
       </c>
       <c r="K6" s="5">
         <v>19.7</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="15">
+        <f t="shared" si="0"/>
+        <v>3.6842105263157857E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1"/>
@@ -788,6 +865,15 @@
       <c r="K8" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="O8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:18" ht="30.75" thickBot="1">
       <c r="A9" s="4" t="s">
@@ -811,6 +897,17 @@
       <c r="K9" s="5">
         <v>273.8</v>
       </c>
+      <c r="O9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="15">
+        <f t="shared" ref="P9:P11" si="2">ABS((B9-J9)/B9)</f>
+        <v>0.25446808510638302</v>
+      </c>
+      <c r="Q9" s="15">
+        <f t="shared" ref="Q9:Q11" si="3">ABS((C9-K9)/C9)</f>
+        <v>9.5200000000000048E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:18" ht="45.75" thickBot="1">
       <c r="A10" s="4" t="s">
@@ -831,6 +928,15 @@
       <c r="K10" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="O10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:18" ht="75.75" thickBot="1">
       <c r="A11" s="4" t="s">
@@ -850,6 +956,15 @@
       </c>
       <c r="K11" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="109.5" customHeight="1">
@@ -871,9 +986,9 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1"/>
@@ -892,6 +1007,13 @@
       <c r="K14" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:18" ht="45.75" thickBot="1">
       <c r="A15" s="4" t="s">
@@ -915,6 +1037,17 @@
       <c r="K15" s="5">
         <v>2.4</v>
       </c>
+      <c r="O15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="15">
+        <f t="shared" ref="P15:P18" si="4">ABS((B15-J15)/B15)</f>
+        <v>3.3333333333333361E-2</v>
+      </c>
+      <c r="Q15" s="15">
+        <f t="shared" ref="Q15:Q18" si="5">ABS((C15-K15)/C15)</f>
+        <v>0.6</v>
+      </c>
     </row>
     <row r="16" spans="1:18" ht="60.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -935,8 +1068,19 @@
       <c r="K16" s="5">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="15">
+        <f t="shared" si="4"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Q16" s="15">
+        <f t="shared" si="5"/>
+        <v>9.3922651933701806E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="75.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -959,8 +1103,19 @@
       <c r="K17" s="5">
         <v>3.68</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="60.75" thickBot="1">
+      <c r="O17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" s="15">
+        <f t="shared" si="4"/>
+        <v>0.94285714285714317</v>
+      </c>
+      <c r="Q17" s="15">
+        <f t="shared" si="5"/>
+        <v>0.21702127659574469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="60.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -981,9 +1136,20 @@
       <c r="K18" s="5">
         <v>2.81</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1">
+      <c r="O18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="15">
+        <f t="shared" si="4"/>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="Q18" s="15">
+        <f t="shared" si="5"/>
+        <v>6.3333333333333311E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
         <v>1</v>
@@ -998,8 +1164,15 @@
       <c r="K20" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O20" s="2"/>
+      <c r="P20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="45.75" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1021,8 +1194,19 @@
       <c r="K21" s="5">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="60.75" thickBot="1">
+      <c r="O21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" s="15">
+        <f t="shared" ref="P21:P24" si="6">ABS((B21-J21)/B21)</f>
+        <v>3.3333333333333361E-2</v>
+      </c>
+      <c r="Q21" s="15">
+        <f t="shared" ref="Q21:Q24" si="7">ABS((C21-K21)/C21)</f>
+        <v>0.18195956454121306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="60.75" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -1041,8 +1225,19 @@
       <c r="K22" s="5">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="15">
+        <f t="shared" si="6"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Q22" s="15">
+        <f t="shared" si="7"/>
+        <v>0.28472222222222221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="75.75" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
@@ -1061,8 +1256,19 @@
       <c r="K23" s="5">
         <v>4.6399999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="60.75" thickBot="1">
+      <c r="O23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23" s="15">
+        <f t="shared" si="6"/>
+        <v>0.94285714285714317</v>
+      </c>
+      <c r="Q23" s="15">
+        <f t="shared" si="7"/>
+        <v>0.32571428571428562</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="60.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -1081,9 +1287,20 @@
       <c r="K24" s="5">
         <v>3.41</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="15">
+        <f t="shared" si="6"/>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="Q24" s="15">
+        <f t="shared" si="7"/>
+        <v>0.36400000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="26" spans="1:17" ht="45.75" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1102,8 +1319,17 @@
       <c r="K26" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="30.75" thickBot="1">
+      <c r="O26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="30.75" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -1125,9 +1351,20 @@
       <c r="K27" s="5">
         <v>3334.1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1">
+      <c r="O27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="15">
+        <f t="shared" ref="P27:Q27" si="8">ABS((B27-J27)/B27)</f>
+        <v>7.1658986175115208E-2</v>
+      </c>
+      <c r="Q27" s="15">
+        <f t="shared" si="8"/>
+        <v>0.27694369973190347</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
         <v>1</v>
@@ -1142,8 +1379,15 @@
       <c r="K29" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O29" s="2"/>
+      <c r="P29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="75.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1165,8 +1409,19 @@
       <c r="K30" s="5">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="90.75" thickBot="1">
+      <c r="O30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P30" s="15">
+        <f t="shared" ref="P30:P35" si="9">ABS((B30-J30)/B30)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="15">
+        <f t="shared" ref="Q30:Q35" si="10">ABS((C30-K30)/C30)</f>
+        <v>3.8834951456310676E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="90.75" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1185,8 +1440,19 @@
       <c r="K31" s="5">
         <v>64.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P31" s="15">
+        <f t="shared" si="9"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q31" s="15">
+        <f t="shared" si="10"/>
+        <v>2.727272727272723E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="45.75" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -1204,6 +1470,17 @@
       </c>
       <c r="K32" s="5">
         <v>1.6</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P32" s="15">
+        <f t="shared" si="9"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="Q32" s="15">
+        <f t="shared" si="10"/>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="75.75" thickBot="1">
@@ -1224,6 +1501,17 @@
       </c>
       <c r="K33" s="5">
         <v>22.5</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P33" s="15">
+        <f t="shared" si="9"/>
+        <v>0.13846153846153852</v>
+      </c>
+      <c r="Q33" s="15">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="30.75" thickBot="1">
@@ -1250,6 +1538,17 @@
       <c r="K34" s="5">
         <v>431.8</v>
       </c>
+      <c r="O34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P34" s="15">
+        <f t="shared" si="9"/>
+        <v>2.2999999999999923E-2</v>
+      </c>
+      <c r="Q34" s="15">
+        <f t="shared" si="10"/>
+        <v>0.96272727272727276</v>
+      </c>
     </row>
     <row r="35" spans="1:18" ht="45.75" thickBot="1">
       <c r="A35" s="4" t="s">
@@ -1269,6 +1568,17 @@
       </c>
       <c r="K35" s="5">
         <v>1.29</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P35" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="15">
+        <f t="shared" si="10"/>
+        <v>7.6923076923076988E-3</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1"/>
@@ -1291,6 +1601,15 @@
       <c r="K37" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="O37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:18" ht="30.75" thickBot="1">
       <c r="A38" s="4" t="s">
@@ -1314,6 +1633,17 @@
       <c r="K38" s="5">
         <v>160.1</v>
       </c>
+      <c r="O38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P38" s="15">
+        <f t="shared" ref="P38:P40" si="11">ABS((B38-J38)/B38)</f>
+        <v>3.3653846153846152E-2</v>
+      </c>
+      <c r="Q38" s="15">
+        <f t="shared" ref="Q38:Q40" si="12">ABS((C38-K38)/C38)</f>
+        <v>0.95243902439024386</v>
+      </c>
     </row>
     <row r="39" spans="1:18" ht="45.75" thickBot="1">
       <c r="A39" s="4" t="s">
@@ -1334,6 +1664,17 @@
       <c r="K39" s="5">
         <v>4.9000000000000004</v>
       </c>
+      <c r="O39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" s="15">
+        <f t="shared" si="11"/>
+        <v>1.4492753623188354E-2</v>
+      </c>
+      <c r="Q39" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:18" ht="75.75" thickBot="1">
       <c r="A40" s="4" t="s">
@@ -1353,6 +1694,17 @@
       </c>
       <c r="K40" s="5">
         <v>18.3</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P40" s="15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="15">
+        <f t="shared" si="12"/>
+        <v>1.6666666666666705E-2</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" thickBot="1"/>
@@ -1375,6 +1727,15 @@
       <c r="K42" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="O42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:18" ht="30.75" thickBot="1">
       <c r="A43" s="4" t="s">
@@ -1398,6 +1759,17 @@
       <c r="K43" s="5">
         <v>265</v>
       </c>
+      <c r="O43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P43" s="15">
+        <f t="shared" ref="P43:P45" si="13">ABS((B43-J43)/B43)</f>
+        <v>0.25446808510638302</v>
+      </c>
+      <c r="Q43" s="15">
+        <f t="shared" ref="Q43:Q45" si="14">ABS((C43-K43)/C43)</f>
+        <v>4.7430830039525688E-2</v>
+      </c>
     </row>
     <row r="44" spans="1:18" ht="45.75" thickBot="1">
       <c r="A44" s="4" t="s">
@@ -1418,6 +1790,15 @@
       <c r="K44" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="O44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P44" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q44" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="45" spans="1:18" ht="75.75" thickBot="1">
       <c r="A45" s="4" t="s">
@@ -1437,6 +1818,15 @@
       </c>
       <c r="K45" s="5" t="s">
         <v>38</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q45" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="109.5" customHeight="1">
@@ -1458,9 +1848,9 @@
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
       <c r="R46" s="6"/>
     </row>
     <row r="47" spans="1:18" ht="15.75" thickBot="1"/>
@@ -1479,8 +1869,15 @@
       <c r="K48" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O48" s="2"/>
+      <c r="P48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="45.75" thickBot="1">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
@@ -1502,8 +1899,19 @@
       <c r="K49" s="5">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="60.75" thickBot="1">
+      <c r="O49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P49" s="15">
+        <f t="shared" ref="P49:P52" si="15">ABS((B49-J49)/B49)</f>
+        <v>3.3333333333333361E-2</v>
+      </c>
+      <c r="Q49" s="15">
+        <f t="shared" ref="Q49:Q52" si="16">ABS((C49-K49)/C49)</f>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="60.75" thickBot="1">
       <c r="A50" s="4" t="s">
         <v>9</v>
       </c>
@@ -1522,8 +1930,19 @@
       <c r="K50" s="5">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P50" s="15">
+        <f t="shared" si="15"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Q50" s="15">
+        <f t="shared" si="16"/>
+        <v>8.6021505376343968E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="75.75" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>10</v>
       </c>
@@ -1542,8 +1961,19 @@
       <c r="K51" s="5">
         <v>5.84</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="60.75" thickBot="1">
+      <c r="O51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P51" s="15">
+        <f t="shared" si="15"/>
+        <v>0.94285714285714317</v>
+      </c>
+      <c r="Q51" s="15">
+        <f t="shared" si="16"/>
+        <v>0.24255319148936164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="60.75" thickBot="1">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -1562,9 +1992,20 @@
       <c r="K52" s="5">
         <v>4.42</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="54" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P52" s="15">
+        <f t="shared" si="15"/>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="Q52" s="15">
+        <f t="shared" si="16"/>
+        <v>0.47333333333333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="54" spans="1:17" ht="45.75" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
@@ -1583,8 +2024,17 @@
       <c r="K54" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="30.75" thickBot="1">
+      <c r="O54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="30.75" thickBot="1">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
@@ -1606,9 +2056,20 @@
       <c r="K55" s="5">
         <v>3395.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1">
+      <c r="O55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P55" s="15">
+        <f t="shared" ref="P55:Q55" si="17">ABS((B55-J55)/B55)</f>
+        <v>7.1658986175115208E-2</v>
+      </c>
+      <c r="Q55" s="15">
+        <f t="shared" si="17"/>
+        <v>0.10918000653381242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="57" spans="1:17" ht="15.75" thickBot="1">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="s">
         <v>1</v>
@@ -1623,8 +2084,15 @@
       <c r="K57" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O57" s="2"/>
+      <c r="P57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="75.75" thickBot="1">
       <c r="A58" s="4" t="s">
         <v>13</v>
       </c>
@@ -1646,8 +2114,19 @@
       <c r="K58" s="5">
         <v>94.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="90.75" thickBot="1">
+      <c r="O58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P58" s="15">
+        <f t="shared" ref="P58:P63" si="18">ABS((B58-J58)/B58)</f>
+        <v>0</v>
+      </c>
+      <c r="Q58" s="15">
+        <f t="shared" ref="Q58:Q63" si="19">ABS((C58-K58)/C58)</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="90.75" thickBot="1">
       <c r="A59" s="4" t="s">
         <v>14</v>
       </c>
@@ -1666,8 +2145,19 @@
       <c r="K59" s="5">
         <v>60.6</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O59" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P59" s="15">
+        <f t="shared" si="18"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q59" s="15">
+        <f t="shared" si="19"/>
+        <v>1.0000000000000024E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="45.75" thickBot="1">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
@@ -1686,8 +2176,19 @@
       <c r="K60" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="75.75" thickBot="1">
+      <c r="O60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P60" s="15">
+        <f t="shared" si="18"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="Q60" s="15">
+        <f t="shared" si="19"/>
+        <v>0.92735042735042739</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="75.75" thickBot="1">
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
@@ -1706,8 +2207,19 @@
       <c r="K61" s="5">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="30.75" thickBot="1">
+      <c r="O61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P61" s="15">
+        <f t="shared" si="18"/>
+        <v>0.13846153846153852</v>
+      </c>
+      <c r="Q61" s="15">
+        <f t="shared" si="19"/>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="30.75" thickBot="1">
       <c r="A62" s="4" t="s">
         <v>17</v>
       </c>
@@ -1726,8 +2238,19 @@
       <c r="K62" s="5">
         <v>499.4</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="45.75" thickBot="1">
+      <c r="O62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P62" s="15">
+        <f t="shared" si="18"/>
+        <v>2.2999999999999923E-2</v>
+      </c>
+      <c r="Q62" s="15">
+        <f t="shared" si="19"/>
+        <v>0.29463276836158198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="45.75" thickBot="1">
       <c r="A63" s="4" t="s">
         <v>18</v>
       </c>
@@ -1745,6 +2268,17 @@
       </c>
       <c r="K63" s="5">
         <v>1.56</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P63" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="15">
+        <f t="shared" si="19"/>
+        <v>0.52727272727272723</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -1763,7 +2297,10 @@
       <c r="K66" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="A66:K66"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A12:C12"/>

</xml_diff>

<commit_message>
Adding colorcodes to Lab 31
</commit_message>
<xml_diff>
--- a/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
+++ b/31_nephrotic_syndrome/nephrotic_syndrome_data.xlsx
@@ -365,13 +365,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -387,18 +393,335 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -690,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -715,10 +1038,10 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="16"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -774,11 +1097,11 @@
       <c r="O4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="7">
         <f>ABS((B4-J4)/B4)</f>
         <v>3.3653846153846152E-2</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="7">
         <f t="shared" ref="Q4:Q6" si="0">ABS((C4-K4)/C4)</f>
         <v>0.65600000000000003</v>
       </c>
@@ -805,11 +1128,11 @@
       <c r="O5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="7">
         <f t="shared" ref="P5:P6" si="1">ABS((B5-J5)/B5)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="7">
         <f t="shared" si="0"/>
         <v>6.1224489795918324E-2</v>
       </c>
@@ -836,11 +1159,11 @@
       <c r="O6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="7">
         <f t="shared" si="0"/>
         <v>3.6842105263157857E-2</v>
       </c>
@@ -900,12 +1223,12 @@
       <c r="O9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P9" s="15">
-        <f t="shared" ref="P9:P11" si="2">ABS((B9-J9)/B9)</f>
+      <c r="P9" s="7">
+        <f t="shared" ref="P9" si="2">ABS((B9-J9)/B9)</f>
         <v>0.25446808510638302</v>
       </c>
-      <c r="Q9" s="15">
-        <f t="shared" ref="Q9:Q11" si="3">ABS((C9-K9)/C9)</f>
+      <c r="Q9" s="7">
+        <f t="shared" ref="Q9" si="3">ABS((C9-K9)/C9)</f>
         <v>9.5200000000000048E-2</v>
       </c>
     </row>
@@ -931,10 +1254,10 @@
       <c r="O10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -960,10 +1283,10 @@
       <c r="O11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -978,11 +1301,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -1040,11 +1363,11 @@
       <c r="O15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="15">
+      <c r="P15" s="7">
         <f t="shared" ref="P15:P18" si="4">ABS((B15-J15)/B15)</f>
         <v>3.3333333333333361E-2</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q15" s="7">
         <f t="shared" ref="Q15:Q18" si="5">ABS((C15-K15)/C15)</f>
         <v>0.6</v>
       </c>
@@ -1071,11 +1394,11 @@
       <c r="O16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="7">
         <f t="shared" si="4"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="Q16" s="7">
         <f t="shared" si="5"/>
         <v>9.3922651933701806E-2</v>
       </c>
@@ -1090,10 +1413,10 @@
       <c r="C17" s="5">
         <v>4.7</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1106,11 +1429,11 @@
       <c r="O17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P17" s="7">
         <f t="shared" si="4"/>
         <v>0.94285714285714317</v>
       </c>
-      <c r="Q17" s="15">
+      <c r="Q17" s="7">
         <f t="shared" si="5"/>
         <v>0.21702127659574469</v>
       </c>
@@ -1125,8 +1448,8 @@
       <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1139,11 +1462,11 @@
       <c r="O18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="7">
         <f t="shared" si="4"/>
         <v>1.2599999999999998</v>
       </c>
-      <c r="Q18" s="15">
+      <c r="Q18" s="7">
         <f t="shared" si="5"/>
         <v>6.3333333333333311E-2</v>
       </c>
@@ -1197,11 +1520,11 @@
       <c r="O21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P21" s="15">
+      <c r="P21" s="7">
         <f t="shared" ref="P21:P24" si="6">ABS((B21-J21)/B21)</f>
         <v>3.3333333333333361E-2</v>
       </c>
-      <c r="Q21" s="15">
+      <c r="Q21" s="7">
         <f t="shared" ref="Q21:Q24" si="7">ABS((C21-K21)/C21)</f>
         <v>0.18195956454121306</v>
       </c>
@@ -1228,11 +1551,11 @@
       <c r="O22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P22" s="15">
+      <c r="P22" s="7">
         <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="Q22" s="15">
+      <c r="Q22" s="7">
         <f t="shared" si="7"/>
         <v>0.28472222222222221</v>
       </c>
@@ -1259,11 +1582,11 @@
       <c r="O23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="15">
+      <c r="P23" s="7">
         <f t="shared" si="6"/>
         <v>0.94285714285714317</v>
       </c>
-      <c r="Q23" s="15">
+      <c r="Q23" s="7">
         <f t="shared" si="7"/>
         <v>0.32571428571428562</v>
       </c>
@@ -1290,11 +1613,11 @@
       <c r="O24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="7">
         <f t="shared" si="6"/>
         <v>1.2599999999999998</v>
       </c>
-      <c r="Q24" s="15">
+      <c r="Q24" s="7">
         <f t="shared" si="7"/>
         <v>0.36400000000000005</v>
       </c>
@@ -1354,11 +1677,11 @@
       <c r="O27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P27" s="15">
+      <c r="P27" s="7">
         <f t="shared" ref="P27:Q27" si="8">ABS((B27-J27)/B27)</f>
         <v>7.1658986175115208E-2</v>
       </c>
-      <c r="Q27" s="15">
+      <c r="Q27" s="7">
         <f t="shared" si="8"/>
         <v>0.27694369973190347</v>
       </c>
@@ -1412,11 +1735,11 @@
       <c r="O30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P30" s="15">
+      <c r="P30" s="7">
         <f t="shared" ref="P30:P35" si="9">ABS((B30-J30)/B30)</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="15">
+      <c r="Q30" s="7">
         <f t="shared" ref="Q30:Q35" si="10">ABS((C30-K30)/C30)</f>
         <v>3.8834951456310676E-2</v>
       </c>
@@ -1443,11 +1766,11 @@
       <c r="O31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P31" s="15">
+      <c r="P31" s="7">
         <f t="shared" si="9"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="Q31" s="15">
+      <c r="Q31" s="7">
         <f t="shared" si="10"/>
         <v>2.727272727272723E-2</v>
       </c>
@@ -1474,11 +1797,11 @@
       <c r="O32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P32" s="15">
+      <c r="P32" s="7">
         <f t="shared" si="9"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="Q32" s="15">
+      <c r="Q32" s="7">
         <f t="shared" si="10"/>
         <v>0.19999999999999996</v>
       </c>
@@ -1505,11 +1828,11 @@
       <c r="O33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P33" s="15">
+      <c r="P33" s="7">
         <f t="shared" si="9"/>
         <v>0.13846153846153852</v>
       </c>
-      <c r="Q33" s="15">
+      <c r="Q33" s="7">
         <f t="shared" si="10"/>
         <v>0.16666666666666666</v>
       </c>
@@ -1524,11 +1847,11 @@
       <c r="C34" s="5">
         <v>220</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
       <c r="I34" s="4" t="s">
         <v>17</v>
       </c>
@@ -1541,11 +1864,11 @@
       <c r="O34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P34" s="15">
+      <c r="P34" s="7">
         <f t="shared" si="9"/>
         <v>2.2999999999999923E-2</v>
       </c>
-      <c r="Q34" s="15">
+      <c r="Q34" s="7">
         <f t="shared" si="10"/>
         <v>0.96272727272727276</v>
       </c>
@@ -1572,11 +1895,11 @@
       <c r="O35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P35" s="15">
+      <c r="P35" s="7">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Q35" s="15">
+      <c r="Q35" s="7">
         <f t="shared" si="10"/>
         <v>7.6923076923076988E-3</v>
       </c>
@@ -1636,11 +1959,11 @@
       <c r="O38" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P38" s="15">
+      <c r="P38" s="7">
         <f t="shared" ref="P38:P40" si="11">ABS((B38-J38)/B38)</f>
         <v>3.3653846153846152E-2</v>
       </c>
-      <c r="Q38" s="15">
+      <c r="Q38" s="7">
         <f t="shared" ref="Q38:Q40" si="12">ABS((C38-K38)/C38)</f>
         <v>0.95243902439024386</v>
       </c>
@@ -1667,11 +1990,11 @@
       <c r="O39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P39" s="15">
+      <c r="P39" s="7">
         <f t="shared" si="11"/>
         <v>1.4492753623188354E-2</v>
       </c>
-      <c r="Q39" s="15">
+      <c r="Q39" s="7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -1698,11 +2021,11 @@
       <c r="O40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P40" s="15">
+      <c r="P40" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q40" s="15">
+      <c r="Q40" s="7">
         <f t="shared" si="12"/>
         <v>1.6666666666666705E-2</v>
       </c>
@@ -1762,12 +2085,12 @@
       <c r="O43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P43" s="15">
-        <f t="shared" ref="P43:P45" si="13">ABS((B43-J43)/B43)</f>
+      <c r="P43" s="7">
+        <f t="shared" ref="P43" si="13">ABS((B43-J43)/B43)</f>
         <v>0.25446808510638302</v>
       </c>
-      <c r="Q43" s="15">
-        <f t="shared" ref="Q43:Q45" si="14">ABS((C43-K43)/C43)</f>
+      <c r="Q43" s="7">
+        <f t="shared" ref="Q43" si="14">ABS((C43-K43)/C43)</f>
         <v>4.7430830039525688E-2</v>
       </c>
     </row>
@@ -1793,10 +2116,10 @@
       <c r="O44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P44" s="15" t="s">
+      <c r="P44" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q44" s="15" t="s">
+      <c r="Q44" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1822,10 +2145,10 @@
       <c r="O45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="15" t="s">
+      <c r="P45" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q45" s="15" t="s">
+      <c r="Q45" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1840,11 +2163,11 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="10" t="s">
+      <c r="I46" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
@@ -1902,11 +2225,11 @@
       <c r="O49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P49" s="15">
+      <c r="P49" s="7">
         <f t="shared" ref="P49:P52" si="15">ABS((B49-J49)/B49)</f>
         <v>3.3333333333333361E-2</v>
       </c>
-      <c r="Q49" s="15">
+      <c r="Q49" s="7">
         <f t="shared" ref="Q49:Q52" si="16">ABS((C49-K49)/C49)</f>
         <v>0.94117647058823528</v>
       </c>
@@ -1933,11 +2256,11 @@
       <c r="O50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P50" s="15">
+      <c r="P50" s="7">
         <f t="shared" si="15"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="Q50" s="15">
+      <c r="Q50" s="7">
         <f t="shared" si="16"/>
         <v>8.6021505376343968E-2</v>
       </c>
@@ -1964,11 +2287,11 @@
       <c r="O51" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P51" s="15">
+      <c r="P51" s="7">
         <f t="shared" si="15"/>
         <v>0.94285714285714317</v>
       </c>
-      <c r="Q51" s="15">
+      <c r="Q51" s="7">
         <f t="shared" si="16"/>
         <v>0.24255319148936164</v>
       </c>
@@ -1995,11 +2318,11 @@
       <c r="O52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P52" s="15">
+      <c r="P52" s="7">
         <f t="shared" si="15"/>
         <v>1.2599999999999998</v>
       </c>
-      <c r="Q52" s="15">
+      <c r="Q52" s="7">
         <f t="shared" si="16"/>
         <v>0.47333333333333333</v>
       </c>
@@ -2059,11 +2382,11 @@
       <c r="O55" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P55" s="15">
+      <c r="P55" s="7">
         <f t="shared" ref="P55:Q55" si="17">ABS((B55-J55)/B55)</f>
         <v>7.1658986175115208E-2</v>
       </c>
-      <c r="Q55" s="15">
+      <c r="Q55" s="7">
         <f t="shared" si="17"/>
         <v>0.10918000653381242</v>
       </c>
@@ -2117,11 +2440,11 @@
       <c r="O58" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P58" s="15">
+      <c r="P58" s="7">
         <f t="shared" ref="P58:P63" si="18">ABS((B58-J58)/B58)</f>
         <v>0</v>
       </c>
-      <c r="Q58" s="15">
+      <c r="Q58" s="7">
         <f t="shared" ref="Q58:Q63" si="19">ABS((C58-K58)/C58)</f>
         <v>4.5454545454545456E-2</v>
       </c>
@@ -2148,11 +2471,11 @@
       <c r="O59" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P59" s="15">
+      <c r="P59" s="7">
         <f t="shared" si="18"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="Q59" s="15">
+      <c r="Q59" s="7">
         <f t="shared" si="19"/>
         <v>1.0000000000000024E-2</v>
       </c>
@@ -2179,11 +2502,11 @@
       <c r="O60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P60" s="15">
+      <c r="P60" s="7">
         <f t="shared" si="18"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="Q60" s="15">
+      <c r="Q60" s="7">
         <f t="shared" si="19"/>
         <v>0.92735042735042739</v>
       </c>
@@ -2210,11 +2533,11 @@
       <c r="O61" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P61" s="15">
+      <c r="P61" s="7">
         <f t="shared" si="18"/>
         <v>0.13846153846153852</v>
       </c>
-      <c r="Q61" s="15">
+      <c r="Q61" s="7">
         <f t="shared" si="19"/>
         <v>4.5999999999999996</v>
       </c>
@@ -2241,11 +2564,11 @@
       <c r="O62" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P62" s="15">
+      <c r="P62" s="7">
         <f t="shared" si="18"/>
         <v>2.2999999999999923E-2</v>
       </c>
-      <c r="Q62" s="15">
+      <c r="Q62" s="7">
         <f t="shared" si="19"/>
         <v>0.29463276836158198</v>
       </c>
@@ -2272,29 +2595,29 @@
       <c r="O63" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P63" s="15">
+      <c r="P63" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="Q63" s="15">
+      <c r="Q63" s="7">
         <f t="shared" si="19"/>
         <v>0.52727272727272723</v>
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2309,6 +2632,105 @@
     <mergeCell ref="G17:H18"/>
     <mergeCell ref="D34:F34"/>
   </mergeCells>
+  <conditionalFormatting sqref="P4:Q6">
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P9:Q11">
+    <cfRule type="cellIs" dxfId="38" priority="19" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15:Q18">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="18" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P21:Q24">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="16" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P27:Q27">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P30:Q35">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P38:Q40">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P43:Q45">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P49:Q52">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P55:Q55">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P58:Q63">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>